<commit_message>
ajuste do tamanho da linha dos gráficos
</commit_message>
<xml_diff>
--- a/doc/ITUB4cg_3anos.xlsx
+++ b/doc/ITUB4cg_3anos.xlsx
@@ -248,6 +248,9 @@
           <c:tx>
             <c:v>Retornos da Ação</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln w="9525"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -4763,6 +4766,9 @@
           <c:tx>
             <c:v>Retornos do Mercado</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln w="9525"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>

</xml_diff>

<commit_message>
ajusta datas dos graficos
</commit_message>
<xml_diff>
--- a/doc/ITUB4cg_3anos.xlsx
+++ b/doc/ITUB4cg_3anos.xlsx
@@ -9673,7 +9673,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20173,7 +20175,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>